<commit_message>
Minor revisions to portrait version.
</commit_message>
<xml_diff>
--- a/ST2-Vintage.xlsx
+++ b/ST2-Vintage.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-440" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="28800" yWindow="-440" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Version2" sheetId="2" r:id="rId2"/>
+    <sheet name="Version2b" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="237">
   <si>
     <t>Sublime Text Vintage Mode</t>
   </si>
@@ -772,12 +773,27 @@
   <si>
     <t>in .vimrc</t>
   </si>
+  <si>
+    <t>Some commands (e.g., z+M, ctrl+j) require custom</t>
+  </si>
+  <si>
+    <t>{"keys": [";"], "command": "show_overlay", "args": {"overlay": "command_palette"}, context: [{"key": "setting.command_mode"}]},</t>
+  </si>
+  <si>
+    <t>{"keys": ["ctrl+j"], "command": "select_lines", "args": {"forward": true}}, {"keys": ["ctrl+k"], "command": "select_lines", "args": {"forward": false}}</t>
+  </si>
+  <si>
+    <t>{"keys": ["super+shift+o"], "command": "prompt_open_folder"}, {"keys": ["super+shift+r"], "command": "sftp_browse_server"}</t>
+  </si>
+  <si>
+    <t>bindings (see below) and/or VintageEx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -888,6 +904,34 @@
       <sz val="9"/>
       <name val="Open Sans"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Monaco"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Open Sans"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -927,7 +971,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1089,8 +1133,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1172,8 +1296,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1336,8 +1470,80 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1378,6 +1584,11 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1418,6 +1629,11 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2677,8 +2893,8 @@
   </sheetPr>
   <dimension ref="B2:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25:T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3870,4 +4086,1508 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="17.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="6" customWidth="1"/>
+    <col min="6" max="7" width="17.83203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" style="6" customWidth="1"/>
+    <col min="10" max="11" width="17.83203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" customWidth="1"/>
+    <col min="14" max="15" width="16.83203125" customWidth="1"/>
+    <col min="16" max="16" width="2.83203125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" style="6" customWidth="1"/>
+    <col min="18" max="19" width="16.83203125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="16" thickBot="1"/>
+    <row r="2" spans="1:15" ht="18">
+      <c r="A2" s="140" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="78"/>
+      <c r="K2" s="79"/>
+    </row>
+    <row r="3" spans="1:15" ht="16">
+      <c r="A3" s="143"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:15" ht="16">
+      <c r="A4" s="128" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="91" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="91"/>
+      <c r="G4" s="129"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="59"/>
+    </row>
+    <row r="5" spans="1:15" ht="16">
+      <c r="A5" s="128"/>
+      <c r="B5" s="91" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="91"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="93" t="s">
+        <v>224</v>
+      </c>
+      <c r="G5" s="129"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="59"/>
+    </row>
+    <row r="6" spans="1:15" ht="16">
+      <c r="A6" s="130" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="G6" s="129"/>
+      <c r="I6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:15" ht="16">
+      <c r="A7" s="131"/>
+      <c r="B7" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="98"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="87" t="s">
+        <v>226</v>
+      </c>
+      <c r="F7" s="87"/>
+      <c r="G7" s="132"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:15" ht="16">
+      <c r="A8" s="133" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="89" t="s">
+        <v>228</v>
+      </c>
+      <c r="G8" s="132"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:15" ht="17" thickBot="1">
+      <c r="A9" s="134"/>
+      <c r="B9" s="135" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="136"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" s="137"/>
+      <c r="G9" s="138"/>
+      <c r="I9" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
+    </row>
+    <row r="10" spans="1:15" ht="16">
+      <c r="I10" s="60"/>
+      <c r="J10" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="62"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" ht="18">
+      <c r="A11" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="78"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="78"/>
+      <c r="G11" s="79"/>
+    </row>
+    <row r="12" spans="1:15" ht="18">
+      <c r="A12" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
+      <c r="I12" s="77" t="s">
+        <v>207</v>
+      </c>
+      <c r="J12" s="48"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="69"/>
+    </row>
+    <row r="13" spans="1:15" ht="16">
+      <c r="A13" s="55"/>
+      <c r="B13" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="59"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="59"/>
+      <c r="I13" s="55" t="s">
+        <v>208</v>
+      </c>
+      <c r="J13" s="58"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="69"/>
+    </row>
+    <row r="14" spans="1:15" ht="16">
+      <c r="A14" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="E14" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="58" t="s">
+        <v>209</v>
+      </c>
+      <c r="K14" s="59"/>
+      <c r="L14" s="68"/>
+    </row>
+    <row r="15" spans="1:15" ht="16">
+      <c r="A15" s="50"/>
+      <c r="B15" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="K15" s="59"/>
+      <c r="L15" s="68"/>
+    </row>
+    <row r="16" spans="1:15" ht="18">
+      <c r="A16" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="E16" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+      <c r="I16" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="68"/>
+    </row>
+    <row r="17" spans="1:19" ht="18">
+      <c r="A17" s="63"/>
+      <c r="B17" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="59"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="59"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="K17" s="24"/>
+      <c r="L17" s="68"/>
+    </row>
+    <row r="18" spans="1:19" ht="18">
+      <c r="A18" s="63"/>
+      <c r="B18" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="59"/>
+      <c r="E18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="I18" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="J18" s="58"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="68"/>
+    </row>
+    <row r="19" spans="1:19" ht="16">
+      <c r="A19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="24"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="61" t="s">
+        <v>217</v>
+      </c>
+      <c r="K19" s="62"/>
+      <c r="L19" s="68"/>
+    </row>
+    <row r="20" spans="1:19" ht="16">
+      <c r="A20" s="4"/>
+      <c r="B20" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="E20" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="58"/>
+      <c r="G20" s="59"/>
+      <c r="L20" s="68"/>
+    </row>
+    <row r="21" spans="1:19" ht="18">
+      <c r="A21" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="59"/>
+      <c r="I21" s="77" t="s">
+        <v>184</v>
+      </c>
+      <c r="J21" s="80"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="68"/>
+    </row>
+    <row r="22" spans="1:19" ht="16">
+      <c r="A22" s="55"/>
+      <c r="B22" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="59"/>
+      <c r="E22" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30"/>
+      <c r="I22" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="68"/>
+    </row>
+    <row r="23" spans="1:19" ht="16">
+      <c r="A23" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="E23" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="58"/>
+      <c r="G23" s="59"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="K23" s="59"/>
+      <c r="L23" s="68"/>
+    </row>
+    <row r="24" spans="1:19" ht="16">
+      <c r="A24" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="58" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" s="59"/>
+      <c r="I24" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:19" ht="16">
+      <c r="A25" s="55"/>
+      <c r="B25" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="C25" s="59"/>
+      <c r="E25" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="K25" s="24"/>
+      <c r="L25" s="106"/>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="106"/>
+      <c r="Q25" s="106"/>
+      <c r="R25" s="106"/>
+      <c r="S25" s="106"/>
+    </row>
+    <row r="26" spans="1:19" ht="16">
+      <c r="A26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="24"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+    </row>
+    <row r="27" spans="1:19" ht="16">
+      <c r="A27" s="4"/>
+      <c r="B27" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C27" s="24"/>
+      <c r="E27" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" s="58"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="K27" s="59"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+    </row>
+    <row r="28" spans="1:19" ht="18">
+      <c r="A28" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" s="59"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" s="23"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+    </row>
+    <row r="29" spans="1:19" ht="18">
+      <c r="A29" s="55"/>
+      <c r="B29" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="59"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="59"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="K29" s="24"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+    </row>
+    <row r="30" spans="1:19" ht="16">
+      <c r="A30" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
+      <c r="E30" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="J30" s="58"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+    </row>
+    <row r="31" spans="1:19" ht="18">
+      <c r="A31" s="2"/>
+      <c r="B31" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="G31" s="24"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="K31" s="59"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+    </row>
+    <row r="32" spans="1:19" ht="16">
+      <c r="A32" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="E32" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="K32" s="59"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+    </row>
+    <row r="33" spans="1:19" ht="16">
+      <c r="A33" s="55"/>
+      <c r="B33" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="59"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" s="59"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="J33" s="23"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+    </row>
+    <row r="34" spans="1:19" ht="16">
+      <c r="A34" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
+      <c r="E34" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K34" s="24"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+    </row>
+    <row r="35" spans="1:19" ht="18">
+      <c r="A35" s="54"/>
+      <c r="B35" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="K35" s="24"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+    </row>
+    <row r="36" spans="1:19" ht="16">
+      <c r="A36" s="50"/>
+      <c r="B36" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="E36" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" s="65"/>
+      <c r="G36" s="66"/>
+      <c r="I36" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" s="58"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+    </row>
+    <row r="37" spans="1:19" ht="16">
+      <c r="A37" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37" s="58"/>
+      <c r="C37" s="59"/>
+      <c r="E37" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="19"/>
+      <c r="G37" s="20"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="59"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+    </row>
+    <row r="38" spans="1:19" ht="16">
+      <c r="A38" s="67"/>
+      <c r="B38" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="C38" s="62"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="20"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="59"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+    </row>
+    <row r="39" spans="1:19" ht="16">
+      <c r="E39" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="58"/>
+      <c r="G39" s="59"/>
+      <c r="I39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="23"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+    </row>
+    <row r="40" spans="1:19" ht="18">
+      <c r="A40" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="59"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="24"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+    </row>
+    <row r="41" spans="1:19" ht="16">
+      <c r="A41" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" s="58"/>
+      <c r="C41" s="59"/>
+      <c r="E41" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="19"/>
+      <c r="G41" s="20"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" s="24"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+    </row>
+    <row r="42" spans="1:19" ht="16">
+      <c r="A42" s="55"/>
+      <c r="B42" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="C42" s="59"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="33"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+    </row>
+    <row r="43" spans="1:19" ht="16">
+      <c r="A43" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="B43" s="19"/>
+      <c r="C43" s="20"/>
+      <c r="E43" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="F43" s="58"/>
+      <c r="G43" s="59"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+    </row>
+    <row r="44" spans="1:19" ht="18">
+      <c r="A44" s="50"/>
+      <c r="B44" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="G44" s="59"/>
+      <c r="I44" s="77" t="s">
+        <v>213</v>
+      </c>
+      <c r="J44" s="48"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+    </row>
+    <row r="45" spans="1:19" ht="16">
+      <c r="A45" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="58"/>
+      <c r="C45" s="59"/>
+      <c r="E45" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="19"/>
+      <c r="G45" s="20"/>
+      <c r="I45" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="J45" s="56"/>
+      <c r="K45" s="57"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+    </row>
+    <row r="46" spans="1:19" ht="16">
+      <c r="A46" s="55"/>
+      <c r="B46" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="59"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46" s="20"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="K46" s="59"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+    </row>
+    <row r="47" spans="1:19" ht="16">
+      <c r="A47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="23"/>
+      <c r="C47" s="24"/>
+      <c r="E47" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" s="58"/>
+      <c r="G47" s="59"/>
+      <c r="I47" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="J47" s="19"/>
+      <c r="K47" s="20"/>
+    </row>
+    <row r="48" spans="1:19" ht="16">
+      <c r="A48" s="52"/>
+      <c r="B48" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="33"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="58" t="s">
+        <v>221</v>
+      </c>
+      <c r="G48" s="59"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="K48" s="20"/>
+    </row>
+    <row r="49" spans="1:19" ht="16">
+      <c r="E49" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20"/>
+      <c r="I49" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="J49" s="58"/>
+      <c r="K49" s="59"/>
+    </row>
+    <row r="50" spans="1:19" ht="18">
+      <c r="A50" s="77" t="s">
+        <v>185</v>
+      </c>
+      <c r="B50" s="43"/>
+      <c r="C50" s="44"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="G50" s="47"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="K50" s="59"/>
+    </row>
+    <row r="51" spans="1:19" ht="16">
+      <c r="A51" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" s="58"/>
+      <c r="C51" s="59"/>
+      <c r="I51" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J51" s="23"/>
+      <c r="K51" s="24"/>
+    </row>
+    <row r="52" spans="1:19" ht="18">
+      <c r="A52" s="55"/>
+      <c r="B52" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="C52" s="59"/>
+      <c r="E52" s="77" t="s">
+        <v>180</v>
+      </c>
+      <c r="F52" s="43"/>
+      <c r="G52" s="44"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K52" s="24"/>
+    </row>
+    <row r="53" spans="1:19" ht="16">
+      <c r="A53" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53" s="23"/>
+      <c r="C53" s="24"/>
+      <c r="E53" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F53" s="23"/>
+      <c r="G53" s="24"/>
+      <c r="I53" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="J53" s="71"/>
+      <c r="K53" s="72"/>
+    </row>
+    <row r="54" spans="1:19" ht="18">
+      <c r="A54" s="2"/>
+      <c r="B54" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" s="24"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="G54" s="24"/>
+      <c r="I54" s="73"/>
+      <c r="J54" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="K54" s="72"/>
+    </row>
+    <row r="55" spans="1:19" ht="18">
+      <c r="A55" s="3"/>
+      <c r="B55" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" s="33"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="G55" s="33"/>
+      <c r="I55" s="74"/>
+      <c r="J55" s="75" t="s">
+        <v>206</v>
+      </c>
+      <c r="K55" s="76"/>
+    </row>
+    <row r="57" spans="1:19" ht="18">
+      <c r="A57" s="77" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="44"/>
+    </row>
+    <row r="58" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A58" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" s="109"/>
+      <c r="C58" s="109"/>
+      <c r="D58" s="109"/>
+      <c r="E58" s="109"/>
+      <c r="F58" s="109"/>
+      <c r="G58" s="109"/>
+      <c r="H58" s="109"/>
+      <c r="I58" s="109"/>
+      <c r="J58" s="109"/>
+      <c r="K58" s="110"/>
+      <c r="L58" s="111"/>
+      <c r="P58" s="111"/>
+      <c r="Q58" s="111"/>
+      <c r="R58" s="111"/>
+      <c r="S58" s="111"/>
+    </row>
+    <row r="59" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A59" s="108"/>
+      <c r="B59" s="113" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" s="109"/>
+      <c r="D59" s="109"/>
+      <c r="E59" s="109"/>
+      <c r="F59" s="109"/>
+      <c r="G59" s="109"/>
+      <c r="H59" s="109"/>
+      <c r="I59" s="109"/>
+      <c r="J59" s="109"/>
+      <c r="K59" s="110"/>
+      <c r="L59" s="111"/>
+      <c r="P59" s="111"/>
+      <c r="Q59" s="111"/>
+      <c r="R59" s="111"/>
+      <c r="S59" s="111"/>
+    </row>
+    <row r="60" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A60" s="114" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="115"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="115"/>
+      <c r="E60" s="115"/>
+      <c r="F60" s="115"/>
+      <c r="G60" s="115"/>
+      <c r="H60" s="115"/>
+      <c r="I60" s="115"/>
+      <c r="J60" s="115"/>
+      <c r="K60" s="116"/>
+      <c r="L60" s="111"/>
+      <c r="P60" s="111"/>
+      <c r="Q60" s="111"/>
+      <c r="R60" s="111"/>
+      <c r="S60" s="111"/>
+    </row>
+    <row r="61" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A61" s="114"/>
+      <c r="B61" s="117" t="s">
+        <v>142</v>
+      </c>
+      <c r="C61" s="115"/>
+      <c r="D61" s="115"/>
+      <c r="E61" s="115"/>
+      <c r="F61" s="115"/>
+      <c r="G61" s="115"/>
+      <c r="H61" s="115"/>
+      <c r="I61" s="115"/>
+      <c r="J61" s="115"/>
+      <c r="K61" s="116"/>
+      <c r="L61" s="111"/>
+      <c r="P61" s="111"/>
+      <c r="Q61" s="111"/>
+      <c r="R61" s="111"/>
+      <c r="S61" s="111"/>
+    </row>
+    <row r="62" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A62" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" s="109"/>
+      <c r="C62" s="109"/>
+      <c r="D62" s="109"/>
+      <c r="E62" s="109"/>
+      <c r="F62" s="109"/>
+      <c r="G62" s="109"/>
+      <c r="H62" s="109"/>
+      <c r="I62" s="109"/>
+      <c r="J62" s="109"/>
+      <c r="K62" s="110"/>
+      <c r="L62" s="111"/>
+      <c r="P62" s="111"/>
+      <c r="Q62" s="111"/>
+      <c r="R62" s="111"/>
+      <c r="S62" s="111"/>
+    </row>
+    <row r="63" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A63" s="108"/>
+      <c r="B63" s="113" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="109"/>
+      <c r="D63" s="109"/>
+      <c r="E63" s="109"/>
+      <c r="F63" s="109"/>
+      <c r="G63" s="109"/>
+      <c r="H63" s="109"/>
+      <c r="I63" s="109"/>
+      <c r="J63" s="109"/>
+      <c r="K63" s="110"/>
+      <c r="L63" s="111"/>
+      <c r="P63" s="111"/>
+      <c r="Q63" s="111"/>
+      <c r="R63" s="111"/>
+      <c r="S63" s="111"/>
+    </row>
+    <row r="64" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A64" s="114" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64" s="115"/>
+      <c r="C64" s="115"/>
+      <c r="D64" s="115"/>
+      <c r="E64" s="115"/>
+      <c r="F64" s="115"/>
+      <c r="G64" s="115"/>
+      <c r="H64" s="115"/>
+      <c r="I64" s="115"/>
+      <c r="J64" s="115"/>
+      <c r="K64" s="116"/>
+      <c r="L64" s="111"/>
+      <c r="P64" s="111"/>
+      <c r="Q64" s="111"/>
+      <c r="R64" s="111"/>
+      <c r="S64" s="111"/>
+    </row>
+    <row r="65" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A65" s="114"/>
+      <c r="B65" s="118" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="115"/>
+      <c r="D65" s="115"/>
+      <c r="E65" s="115"/>
+      <c r="F65" s="115"/>
+      <c r="G65" s="115"/>
+      <c r="H65" s="115"/>
+      <c r="I65" s="115"/>
+      <c r="J65" s="115"/>
+      <c r="K65" s="116"/>
+      <c r="L65" s="111"/>
+      <c r="P65" s="111"/>
+      <c r="Q65" s="111"/>
+      <c r="R65" s="111"/>
+      <c r="S65" s="111"/>
+    </row>
+    <row r="66" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A66" s="108" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" s="109"/>
+      <c r="C66" s="109"/>
+      <c r="D66" s="109"/>
+      <c r="E66" s="109"/>
+      <c r="F66" s="109"/>
+      <c r="G66" s="109"/>
+      <c r="H66" s="109"/>
+      <c r="I66" s="109"/>
+      <c r="J66" s="109"/>
+      <c r="K66" s="110"/>
+      <c r="L66" s="111"/>
+      <c r="P66" s="111"/>
+      <c r="Q66" s="111"/>
+      <c r="R66" s="111"/>
+      <c r="S66" s="111"/>
+    </row>
+    <row r="67" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A67" s="108"/>
+      <c r="B67" s="119" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="109"/>
+      <c r="D67" s="109"/>
+      <c r="E67" s="109"/>
+      <c r="F67" s="109"/>
+      <c r="G67" s="109"/>
+      <c r="H67" s="109"/>
+      <c r="I67" s="109"/>
+      <c r="J67" s="109"/>
+      <c r="K67" s="110"/>
+      <c r="L67" s="111"/>
+      <c r="P67" s="111"/>
+      <c r="Q67" s="111"/>
+      <c r="R67" s="111"/>
+      <c r="S67" s="111"/>
+    </row>
+    <row r="68" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A68" s="114" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="115"/>
+      <c r="C68" s="115"/>
+      <c r="D68" s="115"/>
+      <c r="E68" s="115"/>
+      <c r="F68" s="115"/>
+      <c r="G68" s="115"/>
+      <c r="H68" s="115"/>
+      <c r="I68" s="115"/>
+      <c r="J68" s="115"/>
+      <c r="K68" s="116"/>
+      <c r="L68" s="111"/>
+      <c r="P68" s="111"/>
+      <c r="Q68" s="111"/>
+      <c r="R68" s="111"/>
+      <c r="S68" s="111"/>
+    </row>
+    <row r="69" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A69" s="114"/>
+      <c r="B69" s="118" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="118"/>
+      <c r="D69" s="115"/>
+      <c r="E69" s="115"/>
+      <c r="F69" s="115"/>
+      <c r="G69" s="115"/>
+      <c r="H69" s="115"/>
+      <c r="I69" s="115"/>
+      <c r="J69" s="115"/>
+      <c r="K69" s="116"/>
+      <c r="L69" s="111"/>
+      <c r="P69" s="111"/>
+      <c r="Q69" s="111"/>
+      <c r="R69" s="111"/>
+      <c r="S69" s="111"/>
+    </row>
+    <row r="70" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A70" s="108" t="s">
+        <v>148</v>
+      </c>
+      <c r="B70" s="109"/>
+      <c r="C70" s="109"/>
+      <c r="D70" s="109"/>
+      <c r="E70" s="109"/>
+      <c r="F70" s="109"/>
+      <c r="G70" s="109"/>
+      <c r="H70" s="109"/>
+      <c r="I70" s="109"/>
+      <c r="J70" s="109"/>
+      <c r="K70" s="110"/>
+      <c r="L70" s="111"/>
+      <c r="P70" s="111"/>
+      <c r="Q70" s="111"/>
+      <c r="R70" s="111"/>
+      <c r="S70" s="111"/>
+    </row>
+    <row r="71" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A71" s="108"/>
+      <c r="B71" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="109"/>
+      <c r="D71" s="109"/>
+      <c r="E71" s="109"/>
+      <c r="F71" s="109"/>
+      <c r="G71" s="109"/>
+      <c r="H71" s="109"/>
+      <c r="I71" s="109"/>
+      <c r="J71" s="109"/>
+      <c r="K71" s="110"/>
+      <c r="L71" s="111"/>
+      <c r="P71" s="111"/>
+      <c r="Q71" s="111"/>
+      <c r="R71" s="111"/>
+      <c r="S71" s="111"/>
+    </row>
+    <row r="72" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A72" s="124" t="s">
+        <v>152</v>
+      </c>
+      <c r="B72" s="125"/>
+      <c r="C72" s="125"/>
+      <c r="D72" s="125"/>
+      <c r="E72" s="125"/>
+      <c r="F72" s="125"/>
+      <c r="G72" s="125"/>
+      <c r="H72" s="125"/>
+      <c r="I72" s="125"/>
+      <c r="J72" s="125"/>
+      <c r="K72" s="126"/>
+      <c r="L72" s="111"/>
+      <c r="P72" s="111"/>
+      <c r="Q72" s="111"/>
+      <c r="R72" s="111"/>
+      <c r="S72" s="111"/>
+    </row>
+    <row r="73" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A73" s="124"/>
+      <c r="B73" s="127" t="s">
+        <v>233</v>
+      </c>
+      <c r="C73" s="125"/>
+      <c r="D73" s="125"/>
+      <c r="E73" s="125"/>
+      <c r="F73" s="125"/>
+      <c r="G73" s="125"/>
+      <c r="H73" s="125"/>
+      <c r="I73" s="125"/>
+      <c r="J73" s="125"/>
+      <c r="K73" s="126"/>
+      <c r="L73" s="111"/>
+      <c r="P73" s="111"/>
+      <c r="Q73" s="111"/>
+      <c r="R73" s="111"/>
+      <c r="S73" s="111"/>
+    </row>
+    <row r="74" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A74" s="108" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74" s="109"/>
+      <c r="C74" s="109"/>
+      <c r="D74" s="109"/>
+      <c r="E74" s="109"/>
+      <c r="F74" s="109"/>
+      <c r="G74" s="109"/>
+      <c r="H74" s="109"/>
+      <c r="I74" s="109"/>
+      <c r="J74" s="109"/>
+      <c r="K74" s="110"/>
+      <c r="L74" s="111"/>
+      <c r="P74" s="111"/>
+      <c r="Q74" s="111"/>
+      <c r="R74" s="111"/>
+      <c r="S74" s="111"/>
+    </row>
+    <row r="75" spans="1:19" s="112" customFormat="1" ht="12">
+      <c r="A75" s="120"/>
+      <c r="B75" s="121" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75" s="122"/>
+      <c r="D75" s="122"/>
+      <c r="E75" s="122"/>
+      <c r="F75" s="122"/>
+      <c r="G75" s="122"/>
+      <c r="H75" s="122"/>
+      <c r="I75" s="122"/>
+      <c r="J75" s="122"/>
+      <c r="K75" s="123"/>
+      <c r="L75" s="111"/>
+      <c r="P75" s="111"/>
+      <c r="Q75" s="111"/>
+      <c r="R75" s="111"/>
+      <c r="S75" s="111"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G3"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
+  <pageSetup scale="61" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>